<commit_message>
BOM finally up to date!
</commit_message>
<xml_diff>
--- a/stimjim_BOM.xlsx
+++ b/stimjim_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="158">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">1-2834016-2 _TERM_BLK_2P_SIDE_ENT_2.54MM_PCB</t>
   </si>
   <si>
-    <t xml:space="preserve">Screw_Terminal_01x02</t>
+    <t xml:space="preserve">Push_Terminal_01x02</t>
   </si>
   <si>
     <t xml:space="preserve">1-2834016-2 </t>
@@ -331,19 +331,34 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
+    <t xml:space="preserve">RR0816P-103-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RR08P10.0KDCT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">R3,R10</t>
   </si>
   <si>
     <t xml:space="preserve">5k</t>
   </si>
   <si>
-    <t xml:space="preserve">R21,R17,R19,R20,R22,R18</t>
+    <t xml:space="preserve">RT0603DRE075K05L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-2629-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19,R20</t>
   </si>
   <si>
     <t xml:space="preserve">R_1210_3225Metric_Pad1.42x2.65mm_HandSolder</t>
   </si>
   <si>
-    <t xml:space="preserve">R_Small_US</t>
+    <t xml:space="preserve">1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CHV1206-JW-105ELF </t>
   </si>
   <si>
     <t xml:space="preserve">CHV1206-JW-105ELFCT-ND </t>
@@ -355,7 +370,10 @@
     <t xml:space="preserve">C_Disc_D12.5mm_W5.0mm_P10.00mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C_Small</t>
+    <t xml:space="preserve">2.2nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1206C222MGRAC7800</t>
   </si>
   <si>
     <t xml:space="preserve">399-13198-1-ND </t>
@@ -571,7 +589,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,12 +618,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -628,7 +650,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -885,7 +907,7 @@
         <v>1.368</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -901,7 +923,7 @@
       <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="7" t="n">
         <v>885012206070</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -915,7 +937,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -931,7 +953,7 @@
       <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -945,7 +967,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -961,7 +983,7 @@
       <c r="E11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -975,7 +997,7 @@
         <v>8.88</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -991,7 +1013,7 @@
       <c r="E12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="7" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1005,7 +1027,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -1021,7 +1043,7 @@
       <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="7" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -1035,7 +1057,7 @@
         <v>15.68</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -1051,7 +1073,7 @@
       <c r="E14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1068,7 +1090,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -1084,7 +1106,7 @@
       <c r="E15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="7" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -1098,7 +1120,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -1114,7 +1136,7 @@
       <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>77</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -1128,7 +1150,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -1144,7 +1166,7 @@
       <c r="E17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="7" t="s">
         <v>82</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1158,7 +1180,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -1174,7 +1196,7 @@
       <c r="E18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="7" t="s">
         <v>87</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1188,7 +1210,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -1204,7 +1226,7 @@
       <c r="E19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -1218,7 +1240,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -1234,7 +1256,7 @@
       <c r="E20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="7" t="n">
         <v>731375003</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -1248,7 +1270,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -1259,12 +1281,12 @@
         <v>16</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="7" t="s">
         <v>99</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -1275,89 +1297,126 @@
       </c>
       <c r="I21" s="0" t="n">
         <f aca="false">H21*D21</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">H22*D22</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">H23*D23</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>6</v>
+        <v>110</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="0" t="n">
+        <f aca="false">H24*D24</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="D25" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H25" s="4" t="n">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="0" t="n">
+        <f aca="false">H25*D25</f>
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -1366,13 +1425,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>0.11</v>
@@ -1382,12 +1441,12 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>16</v>
@@ -1398,11 +1457,11 @@
       <c r="E27" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>118</v>
+      <c r="F27" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>0.1</v>
@@ -1412,12 +1471,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>24</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
@@ -1426,13 +1485,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>2.73</v>
@@ -1442,12 +1501,12 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>30</v>
@@ -1456,13 +1515,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>2.81</v>
@@ -1472,27 +1531,27 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>2.43</v>
@@ -1501,16 +1560,16 @@
         <f aca="false">H30*D30</f>
         <v>4.86</v>
       </c>
-      <c r="J30" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>27</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>16</v>
@@ -1521,11 +1580,11 @@
       <c r="E31" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>135</v>
+      <c r="F31" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>0.11</v>
@@ -1534,9 +1593,9 @@
         <f aca="false">H31*D31</f>
         <v>0.44</v>
       </c>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>28</v>
       </c>
@@ -1544,19 +1603,19 @@
         <v>89</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D32" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>2.67</v>
@@ -1566,7 +1625,7 @@
         <v>5.34</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>29</v>
       </c>
@@ -1574,19 +1633,19 @@
         <v>89</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D33" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>0.46</v>
@@ -1596,21 +1655,21 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D34" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>24.5</v>
@@ -1622,13 +1681,14 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D35" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="F35" s="7"/>
       <c r="G35" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>6.298</v>
@@ -1638,13 +1698,13 @@
         <v>6.298</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I37" s="0" t="n">
         <f aca="false">SUM(I2:I35)</f>
-        <v>193.686</v>
+        <v>196.366</v>
       </c>
     </row>
   </sheetData>
@@ -1664,27 +1724,25 @@
     <hyperlink ref="G14" r:id="rId13" display="AD5752AREZ-ND "/>
     <hyperlink ref="G15" r:id="rId14" display="AD1582ARTZREEL7CT-ND "/>
     <hyperlink ref="G16" r:id="rId15" display="296-43866-1-ND"/>
-    <hyperlink ref="F17" r:id="rId16" display="5300H5"/>
-    <hyperlink ref="G17" r:id="rId17" display="L20015-ND "/>
-    <hyperlink ref="G18" r:id="rId18" display="ED10535-ND "/>
-    <hyperlink ref="G19" r:id="rId19" display="1568-1443-ND "/>
-    <hyperlink ref="G20" r:id="rId20" display="WM5514-ND"/>
-    <hyperlink ref="G21" r:id="rId21" display="RR08P1.0KDCT-ND "/>
-    <hyperlink ref="G24" r:id="rId22" display="CHV1206-JW-105ELFCT-ND "/>
-    <hyperlink ref="G25" r:id="rId23" display="399-13198-1-ND "/>
-    <hyperlink ref="G26" r:id="rId24" display="RR08P1.8KDCT-ND "/>
-    <hyperlink ref="G27" r:id="rId25" display="RR08P100DCT-ND "/>
-    <hyperlink ref="G28" r:id="rId26" display="AD8276ARZ-ND "/>
-    <hyperlink ref="G29" r:id="rId27" display="296-30238-1-ND "/>
-    <hyperlink ref="G30" r:id="rId28" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="J30" r:id="rId29" display="Alternate part: DG409DY-T1-E3CT-ND "/>
-    <hyperlink ref="G31" r:id="rId30" display="RR08P200DCT-ND "/>
-    <hyperlink ref="F32" r:id="rId31" display="SSQ-124-03-T-S"/>
+    <hyperlink ref="G17" r:id="rId16" display="L20015-ND "/>
+    <hyperlink ref="G18" r:id="rId17" display="ED10535-ND "/>
+    <hyperlink ref="G19" r:id="rId18" display="1568-1443-ND "/>
+    <hyperlink ref="G20" r:id="rId19" display="WM5514-ND"/>
+    <hyperlink ref="G21" r:id="rId20" display="RR08P1.0KDCT-ND "/>
+    <hyperlink ref="G22" r:id="rId21" display="RR08P10.0KDCT-ND "/>
+    <hyperlink ref="G23" r:id="rId22" display="311-2629-1-ND "/>
+    <hyperlink ref="G24" r:id="rId23" display="CHV1206-JW-105ELFCT-ND "/>
+    <hyperlink ref="G25" r:id="rId24" display="399-13198-1-ND "/>
+    <hyperlink ref="G26" r:id="rId25" display="RR08P1.8KDCT-ND "/>
+    <hyperlink ref="G27" r:id="rId26" display="RR08P100DCT-ND "/>
+    <hyperlink ref="G28" r:id="rId27" display="AD8276ARZ-ND "/>
+    <hyperlink ref="G29" r:id="rId28" display="296-30238-1-ND "/>
+    <hyperlink ref="G30" r:id="rId29" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="J30" r:id="rId30" display="Alternate part: DG409DY-T1-E3CT-ND "/>
+    <hyperlink ref="G31" r:id="rId31" display="RR08P200DCT-ND "/>
     <hyperlink ref="G32" r:id="rId32" display="SAM1206-24-ND "/>
-    <hyperlink ref="F33" r:id="rId33" display="PREC024SAAN-RC"/>
-    <hyperlink ref="G33" r:id="rId34" display="S1012EC-24-ND "/>
-    <hyperlink ref="F34" r:id="rId35" display="EXN-23359-SVP"/>
-    <hyperlink ref="G34" r:id="rId36" display="377-2550-ND"/>
+    <hyperlink ref="G33" r:id="rId33" display="S1012EC-24-ND "/>
+    <hyperlink ref="G34" r:id="rId34" display="377-2550-ND"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
replaced terrible 24-pin female header (too tight) with a better 24-pin female header in BOM
</commit_message>
<xml_diff>
--- a/stimjim_BOM.xlsx
+++ b/stimjim_BOM.xlsx
@@ -457,10 +457,10 @@
     <t xml:space="preserve">Female headers</t>
   </si>
   <si>
-    <t xml:space="preserve">SSQ-124-03-T-S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAM1206-24-ND </t>
+    <t xml:space="preserve">PPTC241LFBN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S7022-ND</t>
   </si>
   <si>
     <t xml:space="preserve">24-pin male headers, 2.54mm pitch</t>
@@ -649,8 +649,8 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1618,11 +1618,11 @@
         <v>146</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>2.67</v>
+        <v>1.37</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">H32*D32</f>
-        <v>5.34</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,7 +1704,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I37" s="0" t="n">
         <f aca="false">SUM(I2:I35)</f>
-        <v>196.366</v>
+        <v>193.766</v>
       </c>
     </row>
   </sheetData>
@@ -1740,7 +1740,7 @@
     <hyperlink ref="G30" r:id="rId29" display="DG509BEY-T1-E3CT-ND "/>
     <hyperlink ref="J30" r:id="rId30" display="Alternate part: DG409DY-T1-E3CT-ND "/>
     <hyperlink ref="G31" r:id="rId31" display="RR08P200DCT-ND "/>
-    <hyperlink ref="G32" r:id="rId32" display="SAM1206-24-ND "/>
+    <hyperlink ref="G32" r:id="rId32" display="S7022-ND"/>
     <hyperlink ref="G33" r:id="rId33" display="S1012EC-24-ND "/>
     <hyperlink ref="G34" r:id="rId34" display="377-2550-ND"/>
   </hyperlinks>

</xml_diff>

<commit_message>
regenerated fab files, schematic and layout files, and BOM.
</commit_message>
<xml_diff>
--- a/stimjim_BOM.xlsx
+++ b/stimjim_BOM.xlsx
@@ -325,7 +325,7 @@
     <t xml:space="preserve">RR08P1.0KDCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R8</t>
+    <t xml:space="preserve">R17,R18,R1,R8</t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -649,8 +649,8 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1301,14 +1301,17 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>102</v>
@@ -1324,12 +1327,12 @@
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">H22*D22</f>
-        <v>0.22</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>105</v>
@@ -1358,6 +1361,9 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>109</v>
       </c>
@@ -1385,6 +1391,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>114</v>
       </c>
@@ -1413,7 +1422,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>119</v>
@@ -1443,7 +1452,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>123</v>
@@ -1473,7 +1482,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>126</v>
@@ -1503,7 +1512,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>130</v>
@@ -1533,7 +1542,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>134</v>
@@ -1566,7 +1575,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>140</v>
@@ -1575,7 +1584,7 @@
         <v>16</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>200</v>
@@ -1591,13 +1600,13 @@
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">H31*D31</f>
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="J31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>89</v>
@@ -1625,10 +1634,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>29</v>
-      </c>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
replaced 0.5% resistors in voltage output with 0.1% (updated BOM), changed gain in lib file, added more documentation to stimjimPulser, added manual voltage control mode.
</commit_message>
<xml_diff>
--- a/stimjim_BOM.xlsx
+++ b/stimjim_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Technion Dropbox)\stimjim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6034AD56-4421-422C-B45C-48127800FFD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04C6E4-1645-4FEF-A71D-6685471AED3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="150">
   <si>
     <t>Id</t>
   </si>
@@ -198,12 +198,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>RR0816P-103-D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RR08P10.0KDCT-ND </t>
-  </si>
-  <si>
     <t>R19,R20</t>
   </si>
   <si>
@@ -234,15 +228,6 @@
     <t>R3,R10</t>
   </si>
   <si>
-    <t>5.05k</t>
-  </si>
-  <si>
-    <t>RT0603DRE075K05L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-2629-1-ND </t>
-  </si>
-  <si>
     <t>R5,R12</t>
   </si>
   <si>
@@ -481,29 +466,30 @@
   </si>
   <si>
     <t>At quantity 5, total cost is 32.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P4.99KDBCT-ND </t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>ERA-3AEB4991V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10KDBCT-ND </t>
+  </si>
+  <si>
+    <t>ERA-3AEB103V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -542,8 +528,43 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -565,10 +586,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,46 +599,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -932,7 +961,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -985,7 +1014,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1000,7 +1029,7 @@
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H2">
@@ -1030,7 +1059,7 @@
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H3">
@@ -1057,10 +1086,10 @@
       <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="17" t="s">
         <v>22</v>
       </c>
       <c r="H4">
@@ -1090,10 +1119,10 @@
       <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="21">
         <v>0.92</v>
       </c>
       <c r="I5">
@@ -1120,7 +1149,7 @@
       <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="18" t="s">
         <v>32</v>
       </c>
       <c r="H6">
@@ -1150,7 +1179,7 @@
       <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="H7">
@@ -1180,7 +1209,7 @@
       <c r="F8" s="2">
         <v>731375003</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H8">
@@ -1210,7 +1239,7 @@
       <c r="F9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="17" t="s">
         <v>45</v>
       </c>
       <c r="H9">
@@ -1240,7 +1269,7 @@
       <c r="F10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="17" t="s">
         <v>49</v>
       </c>
       <c r="H10">
@@ -1270,7 +1299,7 @@
       <c r="F11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="18" t="s">
         <v>52</v>
       </c>
       <c r="H11">
@@ -1280,7 +1309,7 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1292,24 +1321,24 @@
       <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>56</v>
+      <c r="F12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="H12">
-        <v>0.11</v>
+        <v>0.35</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0.44</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1317,22 +1346,22 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="3">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H13">
         <v>0.3</v>
@@ -1347,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
@@ -1356,13 +1385,13 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="H14">
         <v>0.8</v>
@@ -1377,29 +1406,29 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>69</v>
+        <v>146</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="H15">
-        <v>0.12</v>
+        <v>0.35</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1407,7 +1436,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
@@ -1419,10 +1448,10 @@
         <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="H16">
         <v>0.1</v>
@@ -1437,22 +1466,22 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="H17">
         <v>0.23</v>
@@ -1467,22 +1496,22 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="H18">
         <v>26.25</v>
@@ -1497,22 +1526,22 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="H19">
         <v>1.37</v>
@@ -1527,22 +1556,22 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="8">
+        <v>82</v>
+      </c>
+      <c r="D20" s="6">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="H20">
         <v>0.46</v>
@@ -1557,22 +1586,22 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>93</v>
+      <c r="E21" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="H21">
         <v>7.4</v>
@@ -1581,33 +1610,33 @@
         <f t="shared" si="0"/>
         <v>14.8</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D22" s="3">
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="H22">
         <v>4.4400000000000004</v>
@@ -1618,57 +1647,57 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>23</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="14" t="s">
+      <c r="B23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="13">
+        <v>2</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="15">
-        <v>2</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" s="13">
+      <c r="F23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="11">
         <v>3.76</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f t="shared" si="0"/>
         <v>7.52</v>
       </c>
-      <c r="J23" s="13"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="H24">
         <v>15.96</v>
@@ -1678,7 +1707,7 @@
         <v>31.92</v>
       </c>
       <c r="J24" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -1686,22 +1715,22 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D25" s="3">
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="H25">
         <v>7.84</v>
@@ -1716,22 +1745,22 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="H26">
         <v>1.76</v>
@@ -1746,22 +1775,22 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="H27">
         <v>11.21</v>
@@ -1776,22 +1805,22 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>123</v>
       </c>
       <c r="H28">
         <v>1.6</v>
@@ -1806,22 +1835,22 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3">
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>127</v>
       </c>
       <c r="H29">
         <v>2.81</v>
@@ -1836,22 +1865,22 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D30" s="3">
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="H30">
         <v>2.4300000000000002</v>
@@ -1860,8 +1889,8 @@
         <f t="shared" si="0"/>
         <v>4.8600000000000003</v>
       </c>
-      <c r="J30" s="7" t="s">
-        <v>138</v>
+      <c r="J30" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -1869,22 +1898,22 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D31" s="3">
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="H31">
         <v>0.48</v>
@@ -1899,19 +1928,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="H32">
         <v>24.5</v>
@@ -1926,14 +1955,14 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H33">
         <v>6.4</v>
@@ -1943,7 +1972,7 @@
         <v>6.4</v>
       </c>
       <c r="J33" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1958,31 +1987,32 @@
     <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="J30" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G31" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G32" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G15" r:id="rId31" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-3AEB4991V/P4.99KDBCT-ND/3075985" xr:uid="{6B417421-8A04-4243-BE03-F0DE3AE4CFBE}"/>
+    <hyperlink ref="G12" r:id="rId32" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-3AEB103V/P10KDBCT-ND/1466076" xr:uid="{AE39CA6C-7228-4AE4-A87D-853F7793AEC2}"/>
+    <hyperlink ref="F12" r:id="rId33" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-3AEB103V/P10KDBCT-ND/1466076" xr:uid="{698B6260-C226-4928-A503-14193B506CEE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId34"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
updated 78L05 regulator to replace obsolete part
</commit_message>
<xml_diff>
--- a/stimjim_BOM.xlsx
+++ b/stimjim_BOM.xlsx
@@ -460,10 +460,10 @@
     <t xml:space="preserve">L78L05_SO8</t>
   </si>
   <si>
-    <t xml:space="preserve">MC78L05ACDX </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC78L05ACDXCT-ND </t>
+    <t xml:space="preserve">MC78L05ACDR2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC78L05ACDR2GOSCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">Enclosure</t>
@@ -494,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -567,6 +567,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -613,7 +620,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -672,6 +679,10 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -752,10 +763,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,11 +774,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="50.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,18 +1744,18 @@
       <c r="E32" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="15" t="s">
         <v>147</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>0.48</v>
+        <v>0.42</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">H32*D32</f>
-        <v>0.96</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,6 +1810,7 @@
         <v>154</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="CL10F104ZO8NNNC"/>
@@ -1831,8 +1845,9 @@
     <hyperlink ref="G30" r:id="rId30" display="296-30238-1-ND "/>
     <hyperlink ref="G31" r:id="rId31" display="DG509BEY-T1-E3CT-ND "/>
     <hyperlink ref="J31" r:id="rId32" display="Alternate part: DG409DY-T1-E3CT-ND "/>
-    <hyperlink ref="G32" r:id="rId33" display="MC78L05ACDXCT-ND "/>
-    <hyperlink ref="G33" r:id="rId34" display="377-2550-ND"/>
+    <hyperlink ref="F32" r:id="rId33" display="MC78L05ACDR2G"/>
+    <hyperlink ref="G32" r:id="rId34" display="MC78L05ACDR2GOSCT-ND"/>
+    <hyperlink ref="G33" r:id="rId35" display="377-2550-ND"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>